<commit_message>
fix(constants): Fixed mapping for H2_STORAGE
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E15CF4-D73A-46DE-A7A0-4028617242D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000ABA20-359F-4225-8138-92A12C5C9535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="240">
   <si>
     <t>Default value</t>
   </si>
@@ -753,6 +753,9 @@
   </si>
   <si>
     <t>Outputs/EnergyScope/Database/HeatDemand/2015_ES_th.csv</t>
+  </si>
+  <si>
+    <t>Price of Ammonia</t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="C315" sqref="C315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,11 +2720,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="25"/>
-      <c r="C188" s="27"/>
-    </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B188" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C188" s="19"/>
+      <c r="D188" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E188" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F188" s="5">
+        <v>76</v>
+      </c>
+    </row>
     <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2800,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1</v>
+        <v>399</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>146</v>
@@ -2815,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>147</v>
@@ -3927,7 +3943,7 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F188 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>

</xml_diff>

<commit_message>
fix(shed_load): lack of shed load interrupts the program
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000ABA20-359F-4225-8138-92A12C5C9535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB31322-1352-48F6-AFF4-DA9D59F961D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -740,9 +740,6 @@
     <t>Curtailment Cost</t>
   </si>
   <si>
-    <t>Simulations/simulation_ES_DS</t>
-  </si>
-  <si>
     <t>Outputs/EnergyScope/Database/TotalLoadValue/##/2015_ES.csv</t>
   </si>
   <si>
@@ -756,6 +753,9 @@
   </si>
   <si>
     <t>Price of Ammonia</t>
+  </si>
+  <si>
+    <t>Simulations/simulation_40000_ElecImport=0</t>
   </si>
 </sst>
 </file>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="C315" sqref="C315"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,7 +1716,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1837,7 +1837,7 @@
         <v>46</v>
       </c>
       <c r="C59" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>86</v>
@@ -2088,7 +2088,7 @@
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>87</v>
@@ -2137,7 +2137,7 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
@@ -2154,7 +2154,7 @@
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>87</v>
@@ -2246,7 +2246,7 @@
         <v>35</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>87</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B188" s="29" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
fix(soft-link): stop condition and some new plotting functions
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB31322-1352-48F6-AFF4-DA9D59F961D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA3BF62-36D8-44D6-A7D1-7DEAE897160F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,7 +755,7 @@
     <t>Price of Ammonia</t>
   </si>
   <si>
-    <t>Simulations/simulation_40000_ElecImport=0</t>
+    <t>Simulations/simulation_37500_ElecImport=0</t>
   </si>
 </sst>
 </file>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>146</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
fix(mapping): ind_heat demand, cleanup of redundant units
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA3BF62-36D8-44D6-A7D1-7DEAE897160F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674E3B42-E05E-46F1-A3DE-A1DE7AD5B3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="F207" sqref="F207"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="F208" sqref="F208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,8 +2815,8 @@
       <c r="E206" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F206" s="5">
-        <v>402</v>
+      <c r="F206" s="24">
+        <v>90000</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>146</v>
@@ -2830,8 +2830,8 @@
       <c r="E207" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F207" s="5">
-        <v>401</v>
+      <c r="F207" s="24">
+        <v>90001</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>147</v>
@@ -3932,7 +3932,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="33">
+  <dataValidations xWindow="547" yWindow="733" count="31">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3962,9 +3962,7 @@
       <formula2>365</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F169:F170" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F205" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F206" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F207" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F205:F207" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="Initial state of charge. It is defined as the % of total storage capacity." sqref="F102" xr:uid="{C22C312A-4C0D-465E-AA40-04829D4E1DD5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="FInal state of charge. It is defined as the % of total storage capacity." sqref="F103" xr:uid="{70E3A2FC-178F-4589-82CF-31382B011A9B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hourly temperature data" prompt="Path to the tempeature time series for each zone._x000a_This is required for heating technologies (e.g. temperature-dependent COP)" sqref="C136" xr:uid="{DCD0DDF5-CAA3-4B00-8005-5B7C31C37DA9}"/>

</xml_diff>

<commit_message>
fix(MTS): initial/final storage SOC now properly mapped between ES-DS
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674E3B42-E05E-46F1-A3DE-A1DE7AD5B3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D873D4D-785A-4498-99C4-EDBCFD7D2122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="F208" sqref="F208"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2014,7 @@
         <v>4</v>
       </c>
       <c r="C101" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(folders): new ES folder structure now properly called within mapping functions
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D873D4D-785A-4498-99C4-EDBCFD7D2122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62D42DB-D235-45A8-A7B5-C72827155E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="F206" sqref="F206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="24">
-        <v>90000</v>
+        <v>401</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>146</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="24">
-        <v>90001</v>
+        <v>402</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
feat(timeseries): new and revised get_timeseries functions with a lot of cleanup
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62D42DB-D235-45A8-A7B5-C72827155E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F8D64A-C738-428A-9765-EC8FB22ECE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="F206" sqref="F206"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2175,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H130" s="11" t="s">
         <v>69</v>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>177.1</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="F205" s="24">
-        <v>100000</v>
+        <v>90000</v>
       </c>
       <c r="H205" s="1" t="s">
         <v>189</v>

</xml_diff>

<commit_message>
fix(get_capacities): Now possible to assign shares of GAS technologies
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F8D64A-C738-428A-9765-EC8FB22ECE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAB907D-798B-45AF-A1F6-C66E5A507DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+      <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,7 +1837,7 @@
         <v>46</v>
       </c>
       <c r="C59" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>86</v>
@@ -1925,7 +1925,7 @@
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>230</v>
+        <v>58</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>64</v>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>100000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>100000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="F172" s="5">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="F205" s="24">
-        <v>90000</v>
+        <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
         <v>189</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="24">
-        <v>402</v>
+        <v>1500</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>147</v>
@@ -3752,7 +3752,7 @@
         <v>217</v>
       </c>
       <c r="F313" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
@@ -3760,13 +3760,13 @@
         <v>98</v>
       </c>
       <c r="C314" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E314" s="22" t="s">
         <v>218</v>
       </c>
       <c r="F314" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
@@ -3774,13 +3774,13 @@
         <v>99</v>
       </c>
       <c r="C315" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E315" s="22" t="s">
         <v>219</v>
       </c>
       <c r="F315" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
@@ -3794,7 +3794,7 @@
         <v>220</v>
       </c>
       <c r="F316" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
@@ -3808,7 +3808,7 @@
         <v>221</v>
       </c>
       <c r="F317" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
@@ -3822,7 +3822,7 @@
         <v>222</v>
       </c>
       <c r="F318" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
@@ -3836,7 +3836,7 @@
         <v>223</v>
       </c>
       <c r="F319" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
@@ -3844,13 +3844,13 @@
         <v>104</v>
       </c>
       <c r="C320" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E320" s="22" t="s">
         <v>224</v>
       </c>
       <c r="F320" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
@@ -3864,7 +3864,7 @@
         <v>225</v>
       </c>
       <c r="F321" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
@@ -3872,7 +3872,7 @@
         <v>226</v>
       </c>
       <c r="F322" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>